<commit_message>
matriz de prueba auditorias
</commit_message>
<xml_diff>
--- a/PAUA/ENTREGABLES/Matriz de Pruebas Roles de Usuario - 1.xlsx
+++ b/PAUA/ENTREGABLES/Matriz de Pruebas Roles de Usuario - 1.xlsx
@@ -653,13 +653,13 @@
     <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-531</t>
   </si>
   <si>
-    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-375</t>
-  </si>
-  <si>
     <t xml:space="preserve">Homologar Mensajes de conformación hay tres diseños diferentes </t>
   </si>
   <si>
     <t xml:space="preserve">Edita registro </t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-375 / https://paua-sfytgenl.atlassian.net/browse/KPAUA-538</t>
   </si>
 </sst>
 </file>
@@ -6672,10 +6672,10 @@
   <dimension ref="A1:N62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="L43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="9" topLeftCell="L10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="M52" sqref="M52"/>
+      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7033,7 +7033,7 @@
         <v>74</v>
       </c>
       <c r="L13" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>171</v>
@@ -7193,7 +7193,7 @@
         <v>16</v>
       </c>
       <c r="H20" s="45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I20" s="23" t="s">
         <v>73</v>
@@ -7839,7 +7839,7 @@
         <v>16</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I47" t="s">
         <v>79</v>
@@ -7848,7 +7848,7 @@
         <v>28</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="N47" s="1">
         <v>45180</v>
@@ -7906,7 +7906,7 @@
         <v>33</v>
       </c>
       <c r="L49" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M49" s="5"/>
       <c r="N49" s="1">
@@ -7954,7 +7954,7 @@
         <v>33</v>
       </c>
       <c r="L51" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M51" s="5"/>
       <c r="N51" s="1">
@@ -8274,7 +8274,7 @@
     <hyperlink ref="M21" r:id="rId7"/>
     <hyperlink ref="M38" r:id="rId8"/>
     <hyperlink ref="M44" r:id="rId9"/>
-    <hyperlink ref="M47" r:id="rId10"/>
+    <hyperlink ref="M47" r:id="rId10" display="https://paua-sfytgenl.atlassian.net/browse/KPAUA-375"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>

</xml_diff>

<commit_message>
Observaciones Admi de Auditorias
</commit_message>
<xml_diff>
--- a/PAUA/ENTREGABLES/Matriz de Pruebas Roles de Usuario - 1.xlsx
+++ b/PAUA/ENTREGABLES/Matriz de Pruebas Roles de Usuario - 1.xlsx
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="4" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="181">
   <si>
     <t>Ambiente QA</t>
   </si>
@@ -660,6 +660,9 @@
   </si>
   <si>
     <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-375 / https://paua-sfytgenl.atlassian.net/browse/KPAUA-538</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-555</t>
   </si>
 </sst>
 </file>
@@ -1035,6 +1038,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1085,12 +1094,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -6147,113 +6150,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="A47:D50" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item h="1" m="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="10"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="11"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Cuenta de Estatus Incidente" fld="11" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="3">
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="11" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="13" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="14" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="11" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
   <location ref="A24:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField dataField="1" showAll="0"/>
@@ -6317,8 +6214,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -6413,6 +6310,112 @@
     </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A47:D50" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item h="1" m="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="10"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="11"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Cuenta de Estatus Incidente" fld="11" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="3">
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -6672,10 +6675,10 @@
   <dimension ref="A1:N62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="L10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6696,94 +6699,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
     </row>
     <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
     </row>
     <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="34" t="s">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
     </row>
     <row r="5" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
@@ -6897,7 +6900,12 @@
         <v>15</v>
       </c>
       <c r="J8" s="20"/>
-      <c r="M8" s="14"/>
+      <c r="L8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>180</v>
+      </c>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -7192,7 +7200,7 @@
       <c r="G20" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="27" t="s">
         <v>178</v>
       </c>
       <c r="I20" s="23" t="s">
@@ -7220,7 +7228,7 @@
       <c r="G21" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="45"/>
+      <c r="H21" s="27"/>
       <c r="I21" s="23" t="s">
         <v>74</v>
       </c>
@@ -7339,7 +7347,7 @@
       <c r="C27" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="44" t="s">
+      <c r="D27" s="28" t="s">
         <v>55</v>
       </c>
       <c r="E27" s="26" t="s">
@@ -7365,7 +7373,7 @@
       <c r="A28" s="26"/>
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
-      <c r="D28" s="44"/>
+      <c r="D28" s="28"/>
       <c r="E28" s="26"/>
       <c r="F28" s="23" t="s">
         <v>62</v>
@@ -7388,7 +7396,7 @@
       <c r="A29" s="26"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
-      <c r="D29" s="44"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="26"/>
       <c r="F29" s="23" t="s">
         <v>63</v>
@@ -7410,7 +7418,7 @@
       <c r="A30" s="26"/>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
-      <c r="D30" s="44"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="26"/>
       <c r="F30" s="23" t="s">
         <v>65</v>
@@ -7432,7 +7440,7 @@
       <c r="A31" s="26"/>
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
-      <c r="D31" s="44"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="26"/>
       <c r="F31" s="23" t="s">
         <v>64</v>
@@ -7454,7 +7462,7 @@
       <c r="A32" s="26"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
-      <c r="D32" s="44"/>
+      <c r="D32" s="28"/>
       <c r="E32" s="26"/>
       <c r="F32" s="23" t="s">
         <v>60</v>
@@ -8215,6 +8223,38 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="E48:E54"/>
+    <mergeCell ref="D48:D54"/>
+    <mergeCell ref="C48:C54"/>
+    <mergeCell ref="A1:N2"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="G3:N4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="E11:E18"/>
+    <mergeCell ref="D11:D18"/>
+    <mergeCell ref="C11:C18"/>
+    <mergeCell ref="B11:B18"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="D19:D26"/>
+    <mergeCell ref="E19:E26"/>
+    <mergeCell ref="C19:C26"/>
+    <mergeCell ref="B19:B26"/>
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="D40:D44"/>
+    <mergeCell ref="C40:C44"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="A33:A39"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="C33:C39"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="D33:D39"/>
     <mergeCell ref="A55:A62"/>
     <mergeCell ref="E33:E39"/>
     <mergeCell ref="B48:B54"/>
@@ -8231,38 +8271,6 @@
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="A45:A47"/>
     <mergeCell ref="E40:E44"/>
-    <mergeCell ref="D40:D44"/>
-    <mergeCell ref="C40:C44"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="A33:A39"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="C33:C39"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="D33:D39"/>
-    <mergeCell ref="D19:D26"/>
-    <mergeCell ref="E19:E26"/>
-    <mergeCell ref="C19:C26"/>
-    <mergeCell ref="B19:B26"/>
-    <mergeCell ref="A19:A26"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="E48:E54"/>
-    <mergeCell ref="D48:D54"/>
-    <mergeCell ref="C48:C54"/>
-    <mergeCell ref="A1:N2"/>
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="E3:F4"/>
-    <mergeCell ref="G3:N4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="E11:E18"/>
-    <mergeCell ref="D11:D18"/>
-    <mergeCell ref="C11:C18"/>
-    <mergeCell ref="B11:B18"/>
-    <mergeCell ref="A11:A18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1"/>
@@ -8275,9 +8283,10 @@
     <hyperlink ref="M38" r:id="rId8"/>
     <hyperlink ref="M44" r:id="rId9"/>
     <hyperlink ref="M47" r:id="rId10" display="https://paua-sfytgenl.atlassian.net/browse/KPAUA-375"/>
+    <hyperlink ref="M8" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">

</xml_diff>